<commit_message>
more changes to electrical emissions and included some interface changes
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Description</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>T25</t>
+  </si>
+  <si>
+    <t>natural gas-fired boiler</t>
   </si>
 </sst>
 </file>
@@ -900,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -998,43 +1001,46 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.8</v>
+      </c>
       <c r="E4" s="2">
-        <v>0.83069999999999999</v>
+        <v>1.403</v>
       </c>
       <c r="F4" s="2">
-        <v>0.10631400000000001</v>
-      </c>
-      <c r="G4" s="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.22</v>
+      </c>
       <c r="H4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="3"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="2">
-        <v>0.176514</v>
+        <v>0.83069999999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>4.3227599999999998E-2</v>
+        <v>0.10631400000000001</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="17" t="s">
@@ -1044,26 +1050,49 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="2">
-        <v>0.17261399999999999</v>
+        <v>0.176514</v>
       </c>
       <c r="F6" s="2">
-        <v>2.7612000000000001</v>
+        <v>4.3227599999999998E-2</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="17" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="2">
+        <v>0.17261399999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.7612000000000001</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removing agricultural bio gas fired  boiler
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Description</t>
   </si>
@@ -218,18 +218,6 @@
   </si>
   <si>
     <t>DH</t>
-  </si>
-  <si>
-    <t>district heating - bio gas-fired boiler</t>
-  </si>
-  <si>
-    <t>T23</t>
-  </si>
-  <si>
-    <t>district heating - agricultural bio gas-fired boiler</t>
-  </si>
-  <si>
-    <t>T24</t>
   </si>
   <si>
     <t>district heating - natural gas-fired boiler</t>
@@ -903,10 +891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1001,7 +989,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1039,72 +1027,18 @@
         <v>0.8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.83069999999999999</v>
+        <v>0.17261399999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>0.10631400000000001</v>
+        <v>2.7612000000000001</v>
       </c>
       <c r="G5" s="15">
         <v>0.22</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.176514</v>
-      </c>
-      <c r="F6" s="2">
-        <v>4.3227599999999998E-2</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.22</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.17261399999999999</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.7612000000000001</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.22</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1117,7 +1051,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1307,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1449,7 +1383,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1476,7 +1410,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1503,7 +1437,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1530,7 +1464,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing lca linking to database
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -217,12 +217,6 @@
     <t>T10</t>
   </si>
   <si>
-    <t>DH</t>
-  </si>
-  <si>
-    <t>district heating - natural gas-fired boiler</t>
-  </si>
-  <si>
     <t>T25</t>
   </si>
   <si>
@@ -230,6 +224,9 @@
   </si>
   <si>
     <t>from CEA, costs in USD-2015, except for PEN and CO2, rest are assumptions</t>
+  </si>
+  <si>
+    <t>district cooling - natural gas-fired boiler for absorption chiller</t>
   </si>
 </sst>
 </file>
@@ -891,10 +888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -909,7 +906,7 @@
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -935,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -961,7 +958,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -987,9 +984,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1012,33 +1009,6 @@
       <c r="H4" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.17261399999999999</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.7612000000000001</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.22</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1048,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,7 +1035,7 @@
     <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1117,7 +1087,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1145,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1202,7 +1172,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1231,9 +1201,36 @@
         <v>36</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.17261399999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.7612000000000001</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1383,7 +1380,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1410,7 +1407,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1437,7 +1434,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1464,7 +1461,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more commits finalizing the lca
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reference documentation update 2.0 (previous update was overwritten by new changes)
-updated reference for LCA-infrastructure for SG (Resource)
- PEN and CO2 are from ecoinvent 3.4 (SG), KBOB (CH)
- costs are calculated from CEA
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2865" windowWidth="28800" windowHeight="16260" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2865" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -228,12 +228,6 @@
     <t>SOLAR</t>
   </si>
   <si>
-    <t>from CEA, costs in USD-2015,</t>
-  </si>
-  <si>
-    <t>ecoinvent 3.4 - market for natural gas, burned in gas motor, for storage_GLO_2017_Allocation, cut-off</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
@@ -262,6 +256,15 @@
   </si>
   <si>
     <t>educated guess</t>
+  </si>
+  <si>
+    <t>PEN and CO2 from ecoinvent 3.4 - market for natural gas, burned in gas motor, for storage_GLO_2017_Allocation, cut-off, cost from CEA</t>
+  </si>
+  <si>
+    <t>PEN and CO2 from ecoinvent 3.4 database - market for electricity, medium voltage - SG, convert to MJ, cost from CEA</t>
+  </si>
+  <si>
+    <t>PEN and CO2 zero equivalent due to renewable technology, cost from CEA, costs in USD-2015</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>28</v>
@@ -773,16 +776,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,13 +799,13 @@
         <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="12">
         <v>0.9</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,13 +819,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="9">
         <v>0.7</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +864,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>21</v>
@@ -878,16 +881,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -898,16 +901,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="9">
         <v>0.8</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,13 +924,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="9">
         <v>0.7</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +968,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>23</v>
@@ -982,16 +985,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,13 +1008,13 @@
         <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="8">
         <v>2.7</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1025,13 +1028,13 @@
         <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="8">
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1045,13 +1048,13 @@
         <v>26</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6">
         <v>3.2</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,13 +1068,13 @@
         <v>26</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8">
         <v>2.8</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,16 +1085,16 @@
         <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="9">
         <v>0.8</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>24</v>
@@ -1144,16 +1147,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,13 +1170,13 @@
         <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4">
         <v>0.99</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1187,13 +1190,13 @@
         <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="4">
         <v>0.99</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1206,14 +1209,14 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="123" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1241,7 +1244,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1259,7 +1262,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2">
         <f>1.1767+0.0019487+0.0000015726</f>
@@ -1273,7 +1276,7 @@
         <v>1.6860068259385668E-2</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,7 +1297,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1314,7 +1317,7 @@
         <v>1E-4</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating the electricity cost
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SIN/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2865" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2870" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -738,17 +738,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -768,7 +768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -788,7 +788,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -808,7 +808,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -843,17 +843,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -873,7 +873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -893,7 +893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -913,7 +913,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -947,17 +947,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.453125" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,7 +977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -997,7 +997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1111,15 +1111,15 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1209,17 +1209,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
     <col min="6" max="6" width="123" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1293,14 +1293,14 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="E4" s="2">
-        <f>0.22*0.75</f>
-        <v>0.16500000000000001</v>
+        <f>0.2*0.75</f>
+        <v>0.15000000000000002</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>